<commit_message>
Add workshop transcripts and info need visualisation
</commit_message>
<xml_diff>
--- a/annotation/annotation_schema_cookversational_search_german.xlsx
+++ b/annotation/annotation_schema_cookversational_search_german.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Promotion\CookversationalSearch\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Google Drive\Promotion\CookversationalSearch\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{441873AE-759E-4957-AD6F-D021384E9207}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B8ED35-5396-4A27-8458-4A29C47BE23A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA8BC8C-CB17-4341-84BF-B96DC8599B67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" firstSheet="8" activeTab="12" xr2:uid="{4DA8BC8C-CB17-4341-84BF-B96DC8599B67}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="656">
   <si>
     <t>Definition</t>
   </si>
@@ -356,9 +356,6 @@
     <t>Proper Storage Time explicit</t>
   </si>
   <si>
-    <t>Proper Storage implizit</t>
-  </si>
-  <si>
     <t>Ingredient Type</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>Ingredient Substitution - explicit</t>
   </si>
   <si>
-    <t>Ingredient Substitution - implizit</t>
-  </si>
-  <si>
     <t>Ingredient before substitution</t>
   </si>
   <si>
@@ -563,9 +557,6 @@
     <t>Request for Info Source explicit</t>
   </si>
   <si>
-    <t>Request for Info Source implizit</t>
-  </si>
-  <si>
     <t>Request for Ratings</t>
   </si>
   <si>
@@ -620,9 +611,6 @@
     <t>Request for Recipe Search Success</t>
   </si>
   <si>
-    <t>Recipe selection - explizit</t>
-  </si>
-  <si>
     <t>Recipe selection - implicit</t>
   </si>
   <si>
@@ -641,9 +629,6 @@
     <t>Request for Tips/Suggestions</t>
   </si>
   <si>
-    <t>Request for Tips - Rückversicherung</t>
-  </si>
-  <si>
     <t>Picture Request</t>
   </si>
   <si>
@@ -2000,9 +1985,6 @@
     <t>Navigational Instruction on SERP</t>
   </si>
   <si>
-    <t>System Instrucation - Stop Reading out SERP</t>
-  </si>
-  <si>
     <t>Question regarding experiment</t>
   </si>
   <si>
@@ -2022,6 +2004,24 @@
   </si>
   <si>
     <t>Ingredient Existence in Recipe - implicit</t>
+  </si>
+  <si>
+    <t>Proper Storage implicit</t>
+  </si>
+  <si>
+    <t>Ingredient Substitution - implicit</t>
+  </si>
+  <si>
+    <t>Request for Info Source implicit</t>
+  </si>
+  <si>
+    <t>Request for Tips - Reassurance</t>
+  </si>
+  <si>
+    <t>Recipe selection - explicit</t>
+  </si>
+  <si>
+    <t>System Instruction - Stop Reading out SERP</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B401E1D3-9445-4B4C-A072-A2434CC2F18B}">
   <dimension ref="A1:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2658,7 +2658,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2671,7 +2671,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -2681,37 +2681,37 @@
         <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -2721,7 +2721,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -2731,7 +2731,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
@@ -2741,7 +2741,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -2751,17 +2751,17 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2769,20 +2769,20 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -3722,10 +3722,10 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>0</v>
@@ -3744,10 +3744,10 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -3760,10 +3760,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -3776,10 +3776,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -3792,10 +3792,10 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -3810,10 +3810,10 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -3826,10 +3826,10 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -3842,10 +3842,10 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -3858,10 +3858,10 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -3890,7 +3890,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
@@ -3899,10 +3899,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>0</v>
@@ -3917,14 +3917,14 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -3933,14 +3933,14 @@
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -3949,14 +3949,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -3965,21 +3965,21 @@
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -3991,13 +3991,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -4006,13 +4006,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -4021,14 +4021,14 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4044,8 +4044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F915427E-EB66-4D57-9EE6-CCE54387639F}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4058,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -4074,10 +4074,10 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -4090,10 +4090,10 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -4106,10 +4106,10 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -4118,14 +4118,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -4138,10 +4138,10 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -4150,14 +4150,14 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -4166,25 +4166,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
@@ -4195,13 +4195,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>188</v>
+        <v>654</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4211,13 +4211,13 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -4226,11 +4226,11 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
@@ -4246,10 +4246,10 @@
         <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -4264,10 +4264,10 @@
         <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -4280,10 +4280,10 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="36" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -4313,10 +4313,10 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -4329,10 +4329,10 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -4341,14 +4341,14 @@
         <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -4361,10 +4361,10 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -4373,14 +4373,14 @@
         <v>13</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -4389,14 +4389,14 @@
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -4409,10 +4409,10 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -4437,8 +4437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B0DF86-2410-4906-BE52-F9521CE6C0DA}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4451,7 +4451,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="37" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
@@ -4460,10 +4460,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>0</v>
@@ -4478,14 +4478,14 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -4494,14 +4494,14 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -4510,14 +4510,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -4526,14 +4526,14 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -4542,14 +4542,14 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -4561,13 +4561,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -4576,14 +4576,14 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -4592,14 +4592,14 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4608,14 +4608,14 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -4624,14 +4624,14 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -4640,14 +4640,14 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -4663,7 +4663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EE1575-6DD2-47BE-8FAF-B6DF066CFA3D}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4687,10 +4687,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>0</v>
@@ -4709,10 +4709,10 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -4725,10 +4725,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -4741,10 +4741,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -4753,14 +4753,14 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
@@ -4789,10 +4789,10 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -4807,10 +4807,10 @@
         <v>74</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -4825,10 +4825,10 @@
         <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4843,10 +4843,10 @@
         <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -4859,10 +4859,10 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -4875,10 +4875,10 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -4890,10 +4890,10 @@
         <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -4905,10 +4905,10 @@
         <v>80</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -4921,10 +4921,10 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -4936,10 +4936,10 @@
         <v>82</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -4951,10 +4951,10 @@
         <v>83</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -4970,15 +4970,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE098B1-1A9F-4D55-8585-A671B6D9B9D3}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="B29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="39.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="41" style="1" customWidth="1"/>
     <col min="5" max="5" width="52.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="65.7109375" style="1" customWidth="1"/>
@@ -4999,13 +4999,13 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="7" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
@@ -5025,7 +5025,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -5058,13 +5058,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -5082,10 +5082,10 @@
         <v>87</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -5101,10 +5101,10 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -5116,14 +5116,14 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -5135,14 +5135,14 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -5177,10 +5177,10 @@
         <v>90</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -5195,13 +5195,13 @@
         <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -5217,10 +5217,10 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -5236,10 +5236,10 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -5253,10 +5253,10 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -5270,10 +5270,10 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -5289,10 +5289,10 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -5308,10 +5308,10 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -5325,10 +5325,10 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -5342,7 +5342,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -5359,10 +5359,10 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -5378,10 +5378,10 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -5397,10 +5397,10 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G23" s="3"/>
     </row>
@@ -5416,10 +5416,10 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -5435,10 +5435,10 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -5450,14 +5450,14 @@
         <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>100</v>
+        <v>650</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -5466,15 +5466,15 @@
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -5483,12 +5483,12 @@
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -5501,14 +5501,14 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -5520,14 +5520,14 @@
         <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -5543,10 +5543,10 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -5562,10 +5562,10 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -5574,12 +5574,12 @@
         <v>13</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -5596,10 +5596,10 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -5615,10 +5615,10 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G35" s="3"/>
     </row>
@@ -5630,14 +5630,14 @@
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -5649,14 +5649,14 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -5670,7 +5670,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -5687,10 +5687,10 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="G39" s="3"/>
     </row>
@@ -5702,14 +5702,14 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -5721,14 +5721,14 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>109</v>
+        <v>651</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -5740,14 +5740,14 @@
         <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G42" s="3"/>
     </row>
@@ -5756,15 +5756,15 @@
         <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G43" s="3"/>
     </row>
@@ -5773,12 +5773,12 @@
         <v>13</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -5795,10 +5795,10 @@
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G45" s="3"/>
     </row>
@@ -5814,10 +5814,10 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G46" s="3"/>
     </row>
@@ -5829,14 +5829,14 @@
         <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G47" s="3"/>
     </row>
@@ -5848,14 +5848,14 @@
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="G48" s="3"/>
     </row>
@@ -5864,12 +5864,12 @@
         <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -5882,14 +5882,14 @@
         <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="G50" s="3"/>
     </row>
@@ -5901,7 +5901,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -5919,13 +5919,13 @@
         <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G52" s="3"/>
     </row>
@@ -5940,13 +5940,13 @@
         <v>13</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G53" s="3"/>
     </row>
@@ -5961,13 +5961,13 @@
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -5979,7 +5979,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -5997,13 +5997,13 @@
         <v>13</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="G56" s="3"/>
     </row>
@@ -6018,13 +6018,13 @@
         <v>13</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="G57" s="3"/>
     </row>
@@ -6039,13 +6039,13 @@
         <v>13</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="G58" s="3"/>
     </row>
@@ -6060,13 +6060,13 @@
         <v>13</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -6082,10 +6082,10 @@
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -6101,10 +6101,10 @@
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G61" s="3"/>
     </row>
@@ -6121,7 +6121,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6135,7 +6135,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -6144,13 +6144,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>1</v>
@@ -6162,11 +6162,11 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -6179,13 +6179,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -6197,13 +6197,13 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -6215,13 +6215,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F6" s="3"/>
     </row>
@@ -6233,13 +6233,13 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -6251,13 +6251,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -6269,13 +6269,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -6287,13 +6287,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -6305,13 +6305,13 @@
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -6323,13 +6323,13 @@
         <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -6341,13 +6341,13 @@
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -6359,13 +6359,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -6377,13 +6377,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -6395,13 +6395,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -6410,14 +6410,14 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -6426,14 +6426,14 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -6442,14 +6442,14 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -6458,14 +6458,14 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -6474,14 +6474,14 @@
         <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -6497,8 +6497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A411C0C-28B1-4379-A4D6-C3F45C1C4DE2}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6511,7 +6511,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -6520,10 +6520,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>0</v>
@@ -6538,14 +6538,14 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -6554,14 +6554,14 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -6570,14 +6570,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -6586,14 +6586,14 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -6602,14 +6602,14 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -6618,11 +6618,11 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
@@ -6635,13 +6635,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -6653,13 +6653,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -6668,14 +6668,14 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -6684,14 +6684,14 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -6700,14 +6700,14 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -6747,10 +6747,10 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="15" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>0</v>
@@ -6769,7 +6769,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
@@ -6785,10 +6785,10 @@
         <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -6803,10 +6803,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -6819,7 +6819,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
@@ -6835,10 +6835,10 @@
         <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -6853,10 +6853,10 @@
         <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -6869,10 +6869,10 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
@@ -6901,10 +6901,10 @@
         <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -6919,10 +6919,10 @@
         <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -6935,10 +6935,10 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -6951,10 +6951,10 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -6967,10 +6967,10 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -6983,7 +6983,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
@@ -6999,10 +6999,10 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -7017,10 +7017,10 @@
         <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -7035,10 +7035,10 @@
         <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -7051,7 +7051,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
@@ -7067,10 +7067,10 @@
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -7085,10 +7085,10 @@
         <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -7103,10 +7103,10 @@
         <v>54</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -7119,10 +7119,10 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -7138,8 +7138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EFF3A2-12C7-4554-942E-AC5C50C03C75}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7154,7 +7154,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -7166,16 +7166,16 @@
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="13" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>0</v>
@@ -7190,16 +7190,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -7208,13 +7208,13 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
@@ -7227,15 +7227,15 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -7247,15 +7247,15 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>169</v>
+        <v>652</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -7264,13 +7264,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="2"/>
@@ -7283,15 +7283,15 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -7303,15 +7303,15 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -7323,15 +7323,15 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -7340,16 +7340,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -7358,16 +7358,16 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -7376,16 +7376,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -7394,16 +7394,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -7415,15 +7415,15 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>195</v>
+        <v>653</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -7432,13 +7432,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
@@ -7464,14 +7464,14 @@
         <v>13</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -7483,14 +7483,14 @@
         <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -7506,10 +7506,10 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -7521,15 +7521,15 @@
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -7544,11 +7544,11 @@
         <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
@@ -7565,13 +7565,13 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -7587,13 +7587,13 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -7608,11 +7608,11 @@
         <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
@@ -7631,13 +7631,13 @@
         <v>13</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -7655,13 +7655,13 @@
         <v>13</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -7673,15 +7673,15 @@
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -7693,12 +7693,12 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="2"/>
@@ -7714,14 +7714,14 @@
         <v>13</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -7736,14 +7736,14 @@
         <v>13</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -7755,15 +7755,15 @@
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -7780,7 +7780,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7801,10 +7801,10 @@
     </row>
     <row r="2" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>0</v>
@@ -7823,10 +7823,10 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -7839,10 +7839,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -7855,10 +7855,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -7871,10 +7871,10 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -7887,7 +7887,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
@@ -7903,10 +7903,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -7921,10 +7921,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -7937,10 +7937,10 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -7953,10 +7953,10 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -7969,10 +7969,10 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -7985,10 +7985,10 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -7997,10 +7997,10 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8008,10 +8008,10 @@
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -8027,7 +8027,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8045,7 +8045,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>0</v>
@@ -8063,10 +8063,10 @@
         <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -8078,10 +8078,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -8093,10 +8093,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -8108,10 +8108,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -8123,10 +8123,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -8138,10 +8138,10 @@
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -8153,10 +8153,10 @@
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -8168,10 +8168,10 @@
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E10" s="2"/>
     </row>

</xml_diff>